<commit_message>
Part 4 (financial damage), done.
</commit_message>
<xml_diff>
--- a/Second documents/14. Estimation_Financial_Damage.xlsx
+++ b/Second documents/14. Estimation_Financial_Damage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugopigott/Dropbox/2. Work/Vanuatu National Statistics Office/Disaster Mangement Information System/23. RAP/All Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophile_mt/Desktop/Work/Government of Vanuatu/Second documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3E8102-83D5-1443-97CA-ACBC2C293691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3C350E-1E4A-C44B-851F-37A81C8893D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="760" windowWidth="17940" windowHeight="16940" xr2:uid="{D90494D9-DB17-D64C-B6B6-4EC777956C58}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{D90494D9-DB17-D64C-B6B6-4EC777956C58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Cluster </t>
-  </si>
-  <si>
     <t>Number Schools</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>building</t>
+  </si>
+  <si>
+    <t>Cluster</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -306,15 +306,16 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="2" xr:uid="{35A96A9B-6046-3145-923D-1D3B8191232A}"/>
@@ -338,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -378,7 +379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -484,7 +485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -626,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,7 +638,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,20 +650,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>64</v>
+      <c r="E1" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -673,10 +674,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>1000000</v>
@@ -690,10 +691,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
         <v>5000000</v>
@@ -707,10 +708,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
         <v>10000000</v>
@@ -721,13 +722,13 @@
         <v>2025</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="2">
         <v>100000000</v>
@@ -738,13 +739,13 @@
         <v>2025</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2">
         <v>100000000</v>
@@ -755,13 +756,13 @@
         <v>2025</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="2">
         <v>175000</v>
@@ -772,13 +773,13 @@
         <v>2025</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="2">
         <v>2500000</v>
@@ -789,13 +790,13 @@
         <v>2025</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="2">
         <v>1000</v>
@@ -806,13 +807,13 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2">
         <v>160000</v>
@@ -823,13 +824,13 @@
         <v>2025</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
       </c>
       <c r="E11">
         <v>75</v>
@@ -840,13 +841,13 @@
         <v>2025</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>125</v>
@@ -857,13 +858,13 @@
         <v>2025</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>120</v>
@@ -874,13 +875,13 @@
         <v>2025</v>
       </c>
       <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>40</v>
@@ -891,13 +892,13 @@
         <v>2025</v>
       </c>
       <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>150</v>
@@ -908,13 +909,13 @@
         <v>2025</v>
       </c>
       <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>175</v>
@@ -925,13 +926,13 @@
         <v>2025</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
       <c r="E17">
         <v>60</v>
@@ -942,13 +943,13 @@
         <v>2025</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -959,13 +960,13 @@
         <v>2025</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>560</v>
@@ -976,13 +977,13 @@
         <v>2025</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>1560</v>
@@ -993,13 +994,13 @@
         <v>2025</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21">
         <v>515</v>
@@ -1010,13 +1011,13 @@
         <v>2025</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>1200</v>
@@ -1027,13 +1028,13 @@
         <v>2025</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23">
         <v>225</v>
@@ -1044,13 +1045,13 @@
         <v>2025</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24">
         <v>10000</v>
@@ -1061,13 +1062,13 @@
         <v>2025</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
         <v>36</v>
-      </c>
-      <c r="D25" t="s">
-        <v>37</v>
       </c>
       <c r="E25" s="2">
         <v>70000</v>
@@ -1078,13 +1079,13 @@
         <v>2025</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E26" s="2">
         <v>100000</v>
@@ -1095,13 +1096,13 @@
         <v>2025</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="2">
         <v>80000</v>
@@ -1112,13 +1113,13 @@
         <v>2025</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="2">
         <v>400000</v>
@@ -1129,13 +1130,13 @@
         <v>2025</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E29" s="2">
         <v>300000</v>
@@ -1146,13 +1147,13 @@
         <v>2025</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E30" s="2">
         <v>150000</v>
@@ -1163,13 +1164,13 @@
         <v>2025</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="2">
         <v>600000</v>
@@ -1180,13 +1181,13 @@
         <v>2025</v>
       </c>
       <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>45</v>
-      </c>
-      <c r="D32" t="s">
-        <v>46</v>
       </c>
       <c r="E32" s="2">
         <v>20000000</v>
@@ -1197,13 +1198,13 @@
         <v>2025</v>
       </c>
       <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="C33" t="s">
-        <v>45</v>
-      </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="2">
         <v>3000000</v>
@@ -1214,13 +1215,13 @@
         <v>2025</v>
       </c>
       <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
         <v>44</v>
       </c>
-      <c r="C34" t="s">
-        <v>45</v>
-      </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E34">
         <v>5000000</v>
@@ -1231,13 +1232,13 @@
         <v>2025</v>
       </c>
       <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="s">
-        <v>45</v>
-      </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" s="2">
         <v>12000000</v>
@@ -1251,10 +1252,10 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" s="2">
         <v>1000000</v>
@@ -1268,10 +1269,10 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E37" s="2">
         <v>500000</v>
@@ -1285,10 +1286,10 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
         <v>51</v>
-      </c>
-      <c r="D38" t="s">
-        <v>52</v>
       </c>
       <c r="E38" s="2">
         <v>1000000000</v>
@@ -1302,10 +1303,10 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E39" s="2">
         <v>500000</v>
@@ -1319,10 +1320,10 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E40" s="2">
         <v>15000000</v>
@@ -1336,10 +1337,10 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" t="s">
         <v>54</v>
-      </c>
-      <c r="D41" t="s">
-        <v>55</v>
       </c>
       <c r="E41" s="2">
         <v>120000</v>
@@ -1353,10 +1354,10 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="2">
         <v>130000</v>
@@ -1370,10 +1371,10 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" t="s">
         <v>57</v>
-      </c>
-      <c r="D43" t="s">
-        <v>58</v>
       </c>
       <c r="E43" s="2">
         <v>200000</v>
@@ -1387,10 +1388,10 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
         <v>59</v>
-      </c>
-      <c r="D44" t="s">
-        <v>60</v>
       </c>
       <c r="E44" s="2">
         <v>400000</v>
@@ -1404,10 +1405,10 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E45" s="2">
         <v>60000</v>
@@ -1421,10 +1422,10 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E46" s="2">
         <v>100000</v>
@@ -1438,10 +1439,10 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E47" s="2">
         <v>200000</v>

</xml_diff>